<commit_message>
Code refactoring and data reading from excel
</commit_message>
<xml_diff>
--- a/src/test/resources/exceldata/register.xlsx
+++ b/src/test/resources/exceldata/register.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anil.basudkar\eclipse-workspace\DSAlgo-FourPetal\src\test\resources\exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{263C9D0E-7949-4846-BE22-90A5F22A7964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A050872-BFE0-4AA2-A39D-35414669DB41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F2EE075F-87E4-4C79-9751-A5D945535C74}"/>
   </bookViews>
@@ -489,7 +489,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>